<commit_message>
added rubyXL to the test
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,44 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkytaiho/Desktop/RubyAutomation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20520"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Аркуш1" sheetId="1" r:id="rId4"/>
+    <sheet name="Аркуш1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Search</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Cats</t>
+    <t>Test</t>
   </si>
   <si>
-    <t>3.056</t>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <color theme="1"/>
+      <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Arial"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -47,39 +62,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -140,53 +165,53 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="67000"/>
+                <a:satMod val="105000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="73000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="81000"/>
+                <a:satMod val="109000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="78000"/>
+                <a:satMod val="120000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -221,7 +246,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -244,16 +269,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:shade val="98000"/>
                 <a:satMod val="150000"/>
-                <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:shade val="90000"/>
                 <a:satMod val="130000"/>
-                <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -264,42 +289,150 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="false" summaryRight="false"/>
   </sheetPr>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="A2:D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" customFormat="false" ht="15.75" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="false">
+      <c r="A2" s="0" t="str">
+        <v>Birds</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <v>2022-12-07 09:47:18</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>Birds</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <v>2022-12-07 09:43:50</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="false">
+      <c r="A4" s="0" t="str">
+        <v>Cats</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <v>2022-12-07 09:43:40</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="false">
+      <c r="A5" s="0" t="str">
+        <v>Cats</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <v>2022-12-05 14:49:08</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customFormat="false">
+      <c r="A6" s="0" t="str">
+        <v>Birds</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <v>2022-12-05 14:46:47</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customFormat="false">
+      <c r="A7" s="0" t="str">
+        <v>Cats</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <v>2022-12-05 14:45:42</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="false" ht="13">
+      <c r="A11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="16" spans="3:3" customFormat="false" ht="13">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" customFormat="false" ht="13">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="false" ht="13">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" customFormat="false" ht="13">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" customFormat="false" ht="13">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" customFormat="false" ht="13">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" customFormat="false" ht="13">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" customFormat="false" ht="13">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" customFormat="false" ht="13">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" customFormat="false" ht="15.75" customHeight="1">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" customFormat="false" ht="15.75" customHeight="1">
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>